<commit_message>
Update automatico via Actualizar 06-14-2020 01-03-03
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6D3D2C01-A6BB-4967-B8D6-417FFE4BD490}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0F427CA-26DC-49B4-8F9F-5502D9C6C9C6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="773">
   <si>
     <t>Id_Prov</t>
   </si>
@@ -134,6 +134,9 @@
     <t>Changuinola (Cabecera)</t>
   </si>
   <si>
+    <t>SI</t>
+  </si>
+  <si>
     <t>Guabito</t>
   </si>
   <si>
@@ -159,9 +162,6 @@
   </si>
   <si>
     <t>Chiriquí Grande (Cabecera)</t>
-  </si>
-  <si>
-    <t>SI</t>
   </si>
   <si>
     <t>Miramar</t>
@@ -3375,7 +3375,7 @@
   <slicer name="Cordón Sanitario (SI)" xr10:uid="{23800F20-AFA8-4F10-B9A5-1114DB3DF283}" cache="SegmentaciónDeDatos_Cordón_Sanitario__SI" caption="Cerco Sanitario (SI)" style="SlicerStyleDark1" rowHeight="234950"/>
   <slicer name="Provincia" xr10:uid="{05674A6C-F3DE-4DC0-947A-32D804437B88}" cache="SegmentaciónDeDatos_Provincia" caption="Provincia" columnCount="3" rowHeight="241300"/>
   <slicer name="Distrito" xr10:uid="{94517B6B-4F47-417C-85A6-9D51100AC2B7}" cache="SegmentaciónDeDatos_Distrito" caption="Distrito" startItem="60" columnCount="5" rowHeight="241300"/>
-  <slicer name="Corregimiento" xr10:uid="{BE7F280B-65B0-4B5C-BC71-5D2C93821AB4}" cache="SegmentaciónDeDatos_Corregimiento" caption="Corregimiento" startItem="595" columnCount="5" rowHeight="241300"/>
+  <slicer name="Corregimiento" xr10:uid="{BE7F280B-65B0-4B5C-BC71-5D2C93821AB4}" cache="SegmentaciónDeDatos_Corregimiento" caption="Corregimiento" columnCount="5" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -3719,8 +3719,8 @@
   <dimension ref="A10:P721"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O25" sqref="O25:O30"/>
+      <pane ySplit="10" topLeftCell="F17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O722" sqref="O722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4082,7 +4082,9 @@
       </c>
       <c r="M17" s="7"/>
       <c r="N17" s="8"/>
-      <c r="O17" s="7"/>
+      <c r="O17" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" ht="15.75">
@@ -4114,7 +4116,7 @@
         <v>10203</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K18" s="1">
         <v>9.4860296249389648</v>
@@ -4156,7 +4158,7 @@
         <v>10204</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K19" s="1">
         <v>9.2762298583984375</v>
@@ -4198,7 +4200,7 @@
         <v>10206</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K20" s="1">
         <v>9.4120197296142578</v>
@@ -4240,7 +4242,7 @@
         <v>10207</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K21" s="1">
         <v>9.5335798263549805</v>
@@ -4282,7 +4284,7 @@
         <v>10208</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K22" s="1">
         <v>9.2639398574829102</v>
@@ -4324,7 +4326,7 @@
         <v>10209</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K23" s="1">
         <v>9.3837003707885742</v>
@@ -4366,7 +4368,7 @@
         <v>10210</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K24" s="1">
         <v>9.4179201126098633</v>
@@ -4396,7 +4398,7 @@
         <v>103</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G25" s="1">
         <v>8.9838895797729492</v>
@@ -4408,7 +4410,7 @@
         <v>10301</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K25" s="1">
         <v>8.9332103729248047</v>
@@ -4419,7 +4421,7 @@
       <c r="M25" s="7"/>
       <c r="N25" s="8"/>
       <c r="O25" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P25" s="8"/>
     </row>
@@ -4440,7 +4442,7 @@
         <v>103</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G26" s="1">
         <v>8.9838895797729492</v>
@@ -4463,7 +4465,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="8"/>
       <c r="O26" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P26" s="8"/>
     </row>
@@ -4484,7 +4486,7 @@
         <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G27" s="1">
         <v>8.9838895797729492</v>
@@ -4507,7 +4509,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="8"/>
       <c r="O27" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P27" s="8"/>
     </row>
@@ -4528,7 +4530,7 @@
         <v>103</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G28" s="1">
         <v>8.9838895797729492</v>
@@ -4551,7 +4553,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="8"/>
       <c r="O28" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P28" s="8"/>
     </row>
@@ -4572,7 +4574,7 @@
         <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29" s="1">
         <v>8.9838895797729492</v>
@@ -4595,7 +4597,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="8"/>
       <c r="O29" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P29" s="8"/>
     </row>
@@ -4616,7 +4618,7 @@
         <v>103</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G30" s="1">
         <v>8.9838895797729492</v>
@@ -4639,7 +4641,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="8"/>
       <c r="O30" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P30" s="8"/>
     </row>
@@ -6447,7 +6449,7 @@
       <c r="M73" s="7"/>
       <c r="N73" s="8"/>
       <c r="O73" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P73" s="8"/>
     </row>
@@ -6491,7 +6493,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="8"/>
       <c r="O74" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P74" s="8"/>
     </row>
@@ -6535,7 +6537,7 @@
       <c r="M75" s="7"/>
       <c r="N75" s="8"/>
       <c r="O75" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P75" s="8"/>
     </row>
@@ -6579,7 +6581,7 @@
       <c r="M76" s="7"/>
       <c r="N76" s="8"/>
       <c r="O76" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P76" s="8"/>
     </row>
@@ -6623,7 +6625,7 @@
       <c r="M77" s="7"/>
       <c r="N77" s="8"/>
       <c r="O77" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P77" s="8"/>
     </row>
@@ -6667,7 +6669,7 @@
       <c r="M78" s="7"/>
       <c r="N78" s="8"/>
       <c r="O78" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P78" s="8"/>
     </row>
@@ -6711,7 +6713,7 @@
       <c r="M79" s="7"/>
       <c r="N79" s="8"/>
       <c r="O79" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P79" s="8"/>
     </row>
@@ -6755,7 +6757,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="8"/>
       <c r="O80" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P80" s="8"/>
     </row>
@@ -6799,7 +6801,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="8"/>
       <c r="O81" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P81" s="8"/>
     </row>
@@ -6843,7 +6845,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="8"/>
       <c r="O82" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P82" s="8"/>
     </row>
@@ -6887,7 +6889,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="8"/>
       <c r="O83" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P83" s="8"/>
     </row>
@@ -6931,7 +6933,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="8"/>
       <c r="O84" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P84" s="8"/>
     </row>
@@ -6975,7 +6977,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="8"/>
       <c r="O85" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P85" s="8"/>
     </row>
@@ -7019,7 +7021,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="8"/>
       <c r="O86" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P86" s="8"/>
     </row>
@@ -7063,7 +7065,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="8"/>
       <c r="O87" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P87" s="8"/>
     </row>
@@ -7107,7 +7109,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="8"/>
       <c r="O88" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P88" s="8"/>
     </row>
@@ -7151,7 +7153,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="8"/>
       <c r="O89" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P89" s="8"/>
     </row>
@@ -7195,7 +7197,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="8"/>
       <c r="O90" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P90" s="8"/>
     </row>
@@ -7239,7 +7241,7 @@
       <c r="M91" s="7"/>
       <c r="N91" s="8"/>
       <c r="O91" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P91" s="8"/>
     </row>
@@ -7283,7 +7285,7 @@
       <c r="M92" s="7"/>
       <c r="N92" s="8"/>
       <c r="O92" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P92" s="8"/>
     </row>
@@ -7327,7 +7329,7 @@
       <c r="M93" s="7"/>
       <c r="N93" s="8"/>
       <c r="O93" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P93" s="8"/>
     </row>
@@ -7371,7 +7373,7 @@
       <c r="M94" s="7"/>
       <c r="N94" s="8"/>
       <c r="O94" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P94" s="8"/>
     </row>
@@ -7415,7 +7417,7 @@
       <c r="M95" s="7"/>
       <c r="N95" s="8"/>
       <c r="O95" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P95" s="8"/>
     </row>
@@ -7459,7 +7461,7 @@
       <c r="M96" s="7"/>
       <c r="N96" s="8"/>
       <c r="O96" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P96" s="8"/>
     </row>
@@ -7503,7 +7505,7 @@
       <c r="M97" s="7"/>
       <c r="N97" s="8"/>
       <c r="O97" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P97" s="8"/>
     </row>
@@ -7547,7 +7549,7 @@
       <c r="M98" s="7"/>
       <c r="N98" s="8"/>
       <c r="O98" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P98" s="8"/>
     </row>
@@ -7591,7 +7593,7 @@
       <c r="M99" s="7"/>
       <c r="N99" s="8"/>
       <c r="O99" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P99" s="8"/>
     </row>
@@ -7635,7 +7637,7 @@
       <c r="M100" s="7"/>
       <c r="N100" s="8"/>
       <c r="O100" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P100" s="8"/>
     </row>
@@ -7679,7 +7681,7 @@
       <c r="M101" s="7"/>
       <c r="N101" s="8"/>
       <c r="O101" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P101" s="8"/>
     </row>
@@ -7723,7 +7725,7 @@
       <c r="M102" s="7"/>
       <c r="N102" s="8"/>
       <c r="O102" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P102" s="8"/>
     </row>
@@ -7767,7 +7769,7 @@
       <c r="M103" s="7"/>
       <c r="N103" s="8"/>
       <c r="O103" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P103" s="8"/>
     </row>
@@ -7811,7 +7813,7 @@
       <c r="M104" s="7"/>
       <c r="N104" s="8"/>
       <c r="O104" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P104" s="8"/>
     </row>
@@ -7855,7 +7857,7 @@
       <c r="M105" s="7"/>
       <c r="N105" s="8"/>
       <c r="O105" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P105" s="8"/>
     </row>
@@ -7899,7 +7901,7 @@
       <c r="M106" s="7"/>
       <c r="N106" s="8"/>
       <c r="O106" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P106" s="8"/>
     </row>
@@ -7943,7 +7945,7 @@
       <c r="M107" s="7"/>
       <c r="N107" s="8"/>
       <c r="O107" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P107" s="8"/>
     </row>
@@ -7987,7 +7989,7 @@
       <c r="M108" s="7"/>
       <c r="N108" s="8"/>
       <c r="O108" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P108" s="8"/>
     </row>
@@ -8031,7 +8033,7 @@
       <c r="M109" s="7"/>
       <c r="N109" s="8"/>
       <c r="O109" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P109" s="8"/>
     </row>
@@ -8075,7 +8077,7 @@
       <c r="M110" s="7"/>
       <c r="N110" s="8"/>
       <c r="O110" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P110" s="8"/>
     </row>
@@ -8119,7 +8121,7 @@
       <c r="M111" s="7"/>
       <c r="N111" s="8"/>
       <c r="O111" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P111" s="8"/>
     </row>
@@ -8163,7 +8165,7 @@
       <c r="M112" s="7"/>
       <c r="N112" s="8"/>
       <c r="O112" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P112" s="8"/>
     </row>
@@ -15660,7 +15662,7 @@
         <v>702</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G291" s="1">
         <v>7.6422300338745117</v>
@@ -15702,7 +15704,7 @@
         <v>702</v>
       </c>
       <c r="F292" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G292" s="1">
         <v>7.6422300338745117</v>
@@ -15744,7 +15746,7 @@
         <v>702</v>
       </c>
       <c r="F293" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G293" s="1">
         <v>7.6422300338745117</v>
@@ -15786,7 +15788,7 @@
         <v>702</v>
       </c>
       <c r="F294" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G294" s="1">
         <v>7.6422300338745117</v>
@@ -15828,7 +15830,7 @@
         <v>702</v>
       </c>
       <c r="F295" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G295" s="1">
         <v>7.6422300338745117</v>
@@ -15870,7 +15872,7 @@
         <v>702</v>
       </c>
       <c r="F296" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G296" s="1">
         <v>7.6422300338745117</v>
@@ -15912,7 +15914,7 @@
         <v>702</v>
       </c>
       <c r="F297" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G297" s="1">
         <v>7.6422300338745117</v>
@@ -15954,7 +15956,7 @@
         <v>702</v>
       </c>
       <c r="F298" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G298" s="1">
         <v>7.6422300338745117</v>
@@ -15996,7 +15998,7 @@
         <v>702</v>
       </c>
       <c r="F299" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G299" s="1">
         <v>7.6422300338745117</v>
@@ -16038,7 +16040,7 @@
         <v>702</v>
       </c>
       <c r="F300" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G300" s="1">
         <v>7.6422300338745117</v>
@@ -16080,7 +16082,7 @@
         <v>702</v>
       </c>
       <c r="F301" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G301" s="1">
         <v>7.6422300338745117</v>
@@ -16122,7 +16124,7 @@
         <v>702</v>
       </c>
       <c r="F302" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G302" s="1">
         <v>7.6422300338745117</v>
@@ -16164,7 +16166,7 @@
         <v>702</v>
       </c>
       <c r="F303" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G303" s="1">
         <v>7.6422300338745117</v>
@@ -16206,7 +16208,7 @@
         <v>702</v>
       </c>
       <c r="F304" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G304" s="1">
         <v>7.6422300338745117</v>
@@ -16248,7 +16250,7 @@
         <v>702</v>
       </c>
       <c r="F305" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G305" s="1">
         <v>7.6422300338745117</v>
@@ -16290,7 +16292,7 @@
         <v>702</v>
       </c>
       <c r="F306" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G306" s="1">
         <v>7.6422300338745117</v>
@@ -16332,7 +16334,7 @@
         <v>702</v>
       </c>
       <c r="F307" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G307" s="1">
         <v>7.6422300338745117</v>
@@ -16374,7 +16376,7 @@
         <v>702</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G308" s="1">
         <v>7.6422300338745117</v>
@@ -16416,7 +16418,7 @@
         <v>702</v>
       </c>
       <c r="F309" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G309" s="1">
         <v>7.6422300338745117</v>
@@ -16458,7 +16460,7 @@
         <v>702</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G310" s="1">
         <v>7.6422300338745117</v>
@@ -16500,7 +16502,7 @@
         <v>702</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G311" s="1">
         <v>7.6422300338745117</v>
@@ -16542,7 +16544,7 @@
         <v>702</v>
       </c>
       <c r="F312" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G312" s="1">
         <v>7.6422300338745117</v>
@@ -16584,7 +16586,7 @@
         <v>702</v>
       </c>
       <c r="F313" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G313" s="1">
         <v>7.6422300338745117</v>
@@ -16626,7 +16628,7 @@
         <v>702</v>
       </c>
       <c r="F314" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G314" s="1">
         <v>7.6422300338745117</v>
@@ -18621,13 +18623,13 @@
         <v>-78.925697326660156</v>
       </c>
       <c r="M361" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N361" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O361" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P361" s="8"/>
     </row>
@@ -18669,13 +18671,13 @@
         <v>-78.871299743652344</v>
       </c>
       <c r="M362" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N362" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O362" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P362" s="8"/>
     </row>
@@ -18717,13 +18719,13 @@
         <v>-78.91729736328125</v>
       </c>
       <c r="M363" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N363" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O363" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P363" s="8"/>
     </row>
@@ -18765,13 +18767,13 @@
         <v>-78.93609619140625</v>
       </c>
       <c r="M364" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N364" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O364" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P364" s="8"/>
     </row>
@@ -18813,13 +18815,13 @@
         <v>-79.109397888183594</v>
       </c>
       <c r="M365" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N365" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O365" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P365" s="8"/>
     </row>
@@ -18861,13 +18863,13 @@
         <v>-79.045097351074219</v>
       </c>
       <c r="M366" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N366" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O366" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P366" s="8"/>
     </row>
@@ -18909,13 +18911,13 @@
         <v>-79.077102661132813</v>
       </c>
       <c r="M367" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N367" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O367" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P367" s="8"/>
     </row>
@@ -18957,13 +18959,13 @@
         <v>-78.830001831054688</v>
       </c>
       <c r="M368" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N368" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O368" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P368" s="8"/>
     </row>
@@ -19005,13 +19007,13 @@
         <v>-78.898300170898438</v>
       </c>
       <c r="M369" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N369" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O369" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P369" s="8"/>
     </row>
@@ -19053,13 +19055,13 @@
         <v>-78.831497192382813</v>
       </c>
       <c r="M370" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N370" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O370" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P370" s="8"/>
     </row>
@@ -19101,13 +19103,13 @@
         <v>-79.136802673339844</v>
       </c>
       <c r="M371" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N371" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O371" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P371" s="8"/>
     </row>
@@ -19149,13 +19151,13 @@
         <v>-79.129302978515625</v>
       </c>
       <c r="M372" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N372" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O372" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P372" s="8"/>
     </row>
@@ -19197,13 +19199,13 @@
         <v>-78.991500854492188</v>
       </c>
       <c r="M373" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N373" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O373" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P373" s="8"/>
     </row>
@@ -19245,13 +19247,13 @@
         <v>-78.422698974609375</v>
       </c>
       <c r="M374" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N374" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O374" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P374" s="8"/>
     </row>
@@ -19293,13 +19295,13 @@
         <v>-78.674896240234375</v>
       </c>
       <c r="M375" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N375" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O375" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P375" s="8"/>
     </row>
@@ -19341,13 +19343,13 @@
         <v>-78.501899719238281</v>
       </c>
       <c r="M376" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N376" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O376" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P376" s="8"/>
     </row>
@@ -19389,13 +19391,13 @@
         <v>-78.560203552246094</v>
       </c>
       <c r="M377" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N377" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O377" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P377" s="8"/>
     </row>
@@ -19437,13 +19439,13 @@
         <v>-78.500999450683594</v>
       </c>
       <c r="M378" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N378" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O378" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P378" s="8"/>
     </row>
@@ -19485,13 +19487,13 @@
         <v>-78.441703796386719</v>
       </c>
       <c r="M379" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N379" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O379" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P379" s="8"/>
     </row>
@@ -19533,13 +19535,13 @@
         <v>-78.825798034667969</v>
       </c>
       <c r="M380" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N380" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O380" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P380" s="8"/>
     </row>
@@ -19581,13 +19583,13 @@
         <v>-78.683799743652344</v>
       </c>
       <c r="M381" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N381" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O381" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P381" s="8"/>
     </row>
@@ -19629,13 +19631,13 @@
         <v>-78.510498046875</v>
       </c>
       <c r="M382" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N382" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O382" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P382" s="8"/>
     </row>
@@ -19677,13 +19679,13 @@
         <v>-79.535301208496094</v>
       </c>
       <c r="M383" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N383" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O383" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P383" s="8"/>
     </row>
@@ -19725,13 +19727,13 @@
         <v>-79.544502258300781</v>
       </c>
       <c r="M384" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N384" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O384" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P384" s="8"/>
     </row>
@@ -19773,13 +19775,13 @@
         <v>-79.541297912597656</v>
       </c>
       <c r="M385" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N385" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O385" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P385" s="8"/>
     </row>
@@ -19821,13 +19823,13 @@
         <v>-79.535896301269531</v>
       </c>
       <c r="M386" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N386" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O386" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P386" s="8"/>
     </row>
@@ -19869,13 +19871,13 @@
         <v>-79.539398193359375</v>
       </c>
       <c r="M387" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N387" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O387" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P387" s="8"/>
     </row>
@@ -19917,13 +19919,13 @@
         <v>-79.527801513671875</v>
       </c>
       <c r="M388" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N388" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O388" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P388" s="8"/>
     </row>
@@ -19965,13 +19967,13 @@
         <v>-79.525299072265625</v>
       </c>
       <c r="M389" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N389" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O389" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P389" s="8"/>
     </row>
@@ -20013,13 +20015,13 @@
         <v>-79.513801574707031</v>
       </c>
       <c r="M390" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N390" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O390" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P390" s="8"/>
     </row>
@@ -20061,13 +20063,13 @@
         <v>-79.507896423339844</v>
       </c>
       <c r="M391" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N391" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O391" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P391" s="8"/>
     </row>
@@ -20109,13 +20111,13 @@
         <v>-79.485603332519531</v>
       </c>
       <c r="M392" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N392" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O392" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P392" s="8"/>
     </row>
@@ -20157,13 +20159,13 @@
         <v>-79.493598937988281</v>
       </c>
       <c r="M393" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N393" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O393" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P393" s="8"/>
     </row>
@@ -20205,13 +20207,13 @@
         <v>-79.452102661132813</v>
       </c>
       <c r="M394" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N394" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O394" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P394" s="8"/>
     </row>
@@ -20253,13 +20255,13 @@
         <v>-79.437797546386719</v>
       </c>
       <c r="M395" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N395" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O395" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P395" s="8"/>
     </row>
@@ -20301,13 +20303,13 @@
         <v>-79.571502685546875</v>
       </c>
       <c r="M396" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N396" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O396" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P396" s="8"/>
     </row>
@@ -20349,13 +20351,13 @@
         <v>-79.442001342773438</v>
       </c>
       <c r="M397" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N397" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O397" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P397" s="8"/>
     </row>
@@ -20397,13 +20399,13 @@
         <v>-79.602699279785156</v>
       </c>
       <c r="M398" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N398" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O398" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P398" s="8"/>
     </row>
@@ -20445,13 +20447,13 @@
         <v>-79.55419921875</v>
       </c>
       <c r="M399" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N399" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O399" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P399" s="8"/>
     </row>
@@ -20493,13 +20495,13 @@
         <v>-79.218803405761719</v>
       </c>
       <c r="M400" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N400" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O400" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P400" s="8"/>
     </row>
@@ -20541,13 +20543,13 @@
         <v>-79.329200744628906</v>
       </c>
       <c r="M401" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N401" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O401" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P401" s="8"/>
     </row>
@@ -20589,13 +20591,13 @@
         <v>-79.252998352050781</v>
       </c>
       <c r="M402" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N402" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O402" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P402" s="8"/>
     </row>
@@ -20637,13 +20639,13 @@
         <v>-79.400001525878906</v>
       </c>
       <c r="M403" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N403" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O403" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P403" s="8"/>
     </row>
@@ -20685,13 +20687,13 @@
         <v>-79.417999267578125</v>
       </c>
       <c r="M404" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N404" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O404" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P404" s="8"/>
     </row>
@@ -20733,13 +20735,13 @@
         <v>-79.382003784179688</v>
       </c>
       <c r="M405" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N405" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O405" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P405" s="8"/>
     </row>
@@ -20781,13 +20783,13 @@
         <v>-79.510597229003906</v>
       </c>
       <c r="M406" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N406" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O406" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P406" s="8"/>
     </row>
@@ -20829,13 +20831,13 @@
         <v>-79.4927978515625</v>
       </c>
       <c r="M407" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N407" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O407" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P407" s="8"/>
     </row>
@@ -20877,13 +20879,13 @@
         <v>-79.635597229003906</v>
       </c>
       <c r="M408" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N408" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O408" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P408" s="8"/>
     </row>
@@ -20925,13 +20927,13 @@
         <v>-79.607597351074219</v>
       </c>
       <c r="M409" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N409" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O409" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P409" s="8"/>
     </row>
@@ -20973,13 +20975,13 @@
         <v>-79.514198303222656</v>
       </c>
       <c r="M410" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N410" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O410" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P410" s="8"/>
     </row>
@@ -21021,13 +21023,13 @@
         <v>-79.4989013671875</v>
       </c>
       <c r="M411" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N411" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O411" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P411" s="8"/>
     </row>
@@ -21069,13 +21071,13 @@
         <v>-79.478302001953125</v>
       </c>
       <c r="M412" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N412" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O412" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P412" s="8"/>
     </row>
@@ -21117,13 +21119,13 @@
         <v>-79.496200561523438</v>
       </c>
       <c r="M413" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N413" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O413" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P413" s="8"/>
     </row>
@@ -21165,13 +21167,13 @@
         <v>-79.505996704101563</v>
       </c>
       <c r="M414" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N414" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O414" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P414" s="8"/>
     </row>
@@ -21213,13 +21215,13 @@
         <v>-79.482002258300781</v>
       </c>
       <c r="M415" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N415" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O415" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P415" s="8"/>
     </row>
@@ -21261,13 +21263,13 @@
         <v>-79.490699768066406</v>
       </c>
       <c r="M416" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N416" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O416" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P416" s="8"/>
     </row>
@@ -21309,13 +21311,13 @@
         <v>-79.52130126953125</v>
       </c>
       <c r="M417" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N417" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O417" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P417" s="8"/>
     </row>
@@ -21357,13 +21359,13 @@
         <v>-79.457603454589844</v>
       </c>
       <c r="M418" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N418" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O418" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P418" s="8"/>
     </row>
@@ -21405,13 +21407,13 @@
         <v>-79.549201965332031</v>
       </c>
       <c r="M419" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N419" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O419" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P419" s="8"/>
     </row>
@@ -21453,13 +21455,13 @@
         <v>-79.605697631835938</v>
       </c>
       <c r="M420" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N420" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O420" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P420" s="8"/>
     </row>
@@ -21501,13 +21503,13 @@
         <v>-79.594100952148438</v>
       </c>
       <c r="M421" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N421" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O421" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P421" s="8"/>
     </row>
@@ -28901,7 +28903,7 @@
       <c r="M597" s="7"/>
       <c r="N597" s="8"/>
       <c r="O597" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P597" s="8"/>
     </row>
@@ -28945,7 +28947,7 @@
       <c r="M598" s="7"/>
       <c r="N598" s="8"/>
       <c r="O598" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P598" s="8"/>
     </row>
@@ -28989,7 +28991,7 @@
       <c r="M599" s="7"/>
       <c r="N599" s="8"/>
       <c r="O599" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P599" s="8"/>
     </row>
@@ -29033,7 +29035,7 @@
       <c r="M600" s="7"/>
       <c r="N600" s="8"/>
       <c r="O600" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P600" s="8"/>
     </row>
@@ -30083,13 +30085,13 @@
         <v>-79.418296813964844</v>
       </c>
       <c r="M625" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N625" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O625" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P625" s="8"/>
     </row>
@@ -31265,13 +31267,13 @@
         <v>-79.581001281738281</v>
       </c>
       <c r="M653" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N653" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O653" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P653" s="8"/>
     </row>
@@ -31313,13 +31315,13 @@
         <v>-79.625297546386719</v>
       </c>
       <c r="M654" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N654" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O654" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P654" s="8"/>
     </row>
@@ -31361,13 +31363,13 @@
         <v>-79.732101440429688</v>
       </c>
       <c r="M655" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N655" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O655" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P655" s="8"/>
     </row>
@@ -31409,13 +31411,13 @@
         <v>-79.714302062988281</v>
       </c>
       <c r="M656" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N656" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O656" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P656" s="8"/>
     </row>
@@ -31457,13 +31459,13 @@
         <v>-79.712501525878906</v>
       </c>
       <c r="M657" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N657" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O657" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P657" s="8"/>
     </row>
@@ -31505,13 +31507,13 @@
         <v>-79.758499145507813</v>
       </c>
       <c r="M658" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N658" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O658" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P658" s="8"/>
     </row>
@@ -31553,13 +31555,13 @@
         <v>-79.786201477050781</v>
       </c>
       <c r="M659" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N659" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O659" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P659" s="8"/>
     </row>
@@ -31601,13 +31603,13 @@
         <v>-79.603302001953125</v>
       </c>
       <c r="M660" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N660" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O660" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P660" s="8"/>
     </row>
@@ -31649,13 +31651,13 @@
         <v>-79.691200256347656</v>
       </c>
       <c r="M661" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N661" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O661" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P661" s="8"/>
     </row>
@@ -31697,13 +31699,13 @@
         <v>-79.627899169921875</v>
       </c>
       <c r="M662" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N662" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O662" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P662" s="8"/>
     </row>
@@ -31745,13 +31747,13 @@
         <v>-79.665397644042969</v>
       </c>
       <c r="M663" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N663" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O663" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P663" s="8"/>
     </row>
@@ -31793,13 +31795,13 @@
         <v>-79.680496215820313</v>
       </c>
       <c r="M664" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N664" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O664" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P664" s="8"/>
     </row>
@@ -31841,13 +31843,13 @@
         <v>-79.843696594238281</v>
       </c>
       <c r="M665" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N665" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O665" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P665" s="8"/>
     </row>
@@ -31889,13 +31891,13 @@
         <v>-79.963798522949219</v>
       </c>
       <c r="M666" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N666" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O666" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P666" s="8"/>
     </row>
@@ -31937,13 +31939,13 @@
         <v>-79.871101379394531</v>
       </c>
       <c r="M667" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N667" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O667" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P667" s="8"/>
     </row>
@@ -31985,13 +31987,13 @@
         <v>-79.932403564453125</v>
       </c>
       <c r="M668" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N668" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O668" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P668" s="8"/>
     </row>
@@ -32033,13 +32035,13 @@
         <v>-80.102798461914063</v>
       </c>
       <c r="M669" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N669" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O669" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P669" s="8"/>
     </row>
@@ -32081,13 +32083,13 @@
         <v>-80.090301513671875</v>
       </c>
       <c r="M670" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N670" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O670" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P670" s="8"/>
     </row>
@@ -32129,13 +32131,13 @@
         <v>-80.025596618652344</v>
       </c>
       <c r="M671" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N671" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O671" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P671" s="8"/>
     </row>
@@ -32177,13 +32179,13 @@
         <v>-80.013496398925781</v>
       </c>
       <c r="M672" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N672" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O672" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P672" s="8"/>
     </row>
@@ -32225,13 +32227,13 @@
         <v>-79.905601501464844</v>
       </c>
       <c r="M673" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N673" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O673" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P673" s="8"/>
     </row>
@@ -32273,13 +32275,13 @@
         <v>-79.868896484375</v>
       </c>
       <c r="M674" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N674" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O674" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P674" s="8"/>
     </row>
@@ -32321,13 +32323,13 @@
         <v>-79.862998962402344</v>
       </c>
       <c r="M675" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N675" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O675" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P675" s="8"/>
     </row>
@@ -32369,13 +32371,13 @@
         <v>-80.111801147460938</v>
       </c>
       <c r="M676" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N676" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O676" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P676" s="8"/>
     </row>
@@ -32417,13 +32419,13 @@
         <v>-79.797798156738281</v>
       </c>
       <c r="M677" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N677" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O677" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P677" s="8"/>
     </row>
@@ -32465,13 +32467,13 @@
         <v>-79.849998474121094</v>
       </c>
       <c r="M678" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N678" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O678" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P678" s="8"/>
     </row>
@@ -32513,13 +32515,13 @@
         <v>-79.888397216796875</v>
       </c>
       <c r="M679" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N679" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O679" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P679" s="8"/>
     </row>
@@ -32561,13 +32563,13 @@
         <v>-79.950599670410156</v>
       </c>
       <c r="M680" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N680" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O680" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P680" s="8"/>
     </row>
@@ -32609,13 +32611,13 @@
         <v>-79.955902099609375</v>
       </c>
       <c r="M681" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N681" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O681" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P681" s="8"/>
     </row>
@@ -32657,13 +32659,13 @@
         <v>-79.942596435546875</v>
       </c>
       <c r="M682" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N682" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O682" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P682" s="8"/>
     </row>
@@ -32705,13 +32707,13 @@
         <v>-79.809700012207031</v>
       </c>
       <c r="M683" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N683" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O683" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P683" s="8"/>
     </row>
@@ -32753,13 +32755,13 @@
         <v>-79.91290283203125</v>
       </c>
       <c r="M684" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N684" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O684" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P684" s="8"/>
     </row>
@@ -32801,13 +32803,13 @@
         <v>-79.87860107421875</v>
       </c>
       <c r="M685" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N685" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O685" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P685" s="8"/>
     </row>
@@ -32849,13 +32851,13 @@
         <v>-79.758903503417969</v>
       </c>
       <c r="M686" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N686" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O686" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P686" s="8"/>
     </row>
@@ -32897,13 +32899,13 @@
         <v>-79.875900268554688</v>
       </c>
       <c r="M687" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N687" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O687" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P687" s="8"/>
     </row>
@@ -32945,13 +32947,13 @@
         <v>-80.010101318359375</v>
       </c>
       <c r="M688" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N688" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O688" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P688" s="8"/>
     </row>
@@ -32993,13 +32995,13 @@
         <v>-79.790901184082031</v>
       </c>
       <c r="M689" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N689" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O689" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P689" s="8"/>
     </row>
@@ -33041,13 +33043,13 @@
         <v>-79.765098571777344</v>
       </c>
       <c r="M690" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N690" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O690" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P690" s="8"/>
     </row>
@@ -33089,13 +33091,13 @@
         <v>-79.888198852539063</v>
       </c>
       <c r="M691" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N691" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O691" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P691" s="8"/>
     </row>
@@ -33137,13 +33139,13 @@
         <v>-79.895301818847656</v>
       </c>
       <c r="M692" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N692" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O692" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P692" s="8"/>
     </row>
@@ -33185,13 +33187,13 @@
         <v>-79.957099914550781</v>
       </c>
       <c r="M693" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N693" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O693" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P693" s="8"/>
     </row>
@@ -33233,13 +33235,13 @@
         <v>-79.964401245117188</v>
       </c>
       <c r="M694" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N694" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O694" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P694" s="8"/>
     </row>
@@ -33281,13 +33283,13 @@
         <v>-79.781501770019531</v>
       </c>
       <c r="M695" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N695" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O695" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P695" s="8"/>
     </row>
@@ -33329,13 +33331,13 @@
         <v>-79.804801940917969</v>
       </c>
       <c r="M696" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N696" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O696" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P696" s="8"/>
     </row>
@@ -33377,13 +33379,13 @@
         <v>-79.823799133300781</v>
       </c>
       <c r="M697" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N697" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O697" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P697" s="8"/>
     </row>
@@ -33425,13 +33427,13 @@
         <v>-79.869003295898438</v>
       </c>
       <c r="M698" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N698" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O698" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P698" s="8"/>
     </row>
@@ -33473,13 +33475,13 @@
         <v>-79.827598571777344</v>
       </c>
       <c r="M699" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N699" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O699" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P699" s="8"/>
     </row>
@@ -33521,13 +33523,13 @@
         <v>-79.840896606445313</v>
       </c>
       <c r="M700" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N700" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O700" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P700" s="8"/>
     </row>
@@ -33569,13 +33571,13 @@
         <v>-79.891098022460938</v>
       </c>
       <c r="M701" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N701" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O701" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P701" s="8"/>
     </row>
@@ -33617,13 +33619,13 @@
         <v>-79.9302978515625</v>
       </c>
       <c r="M702" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N702" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O702" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P702" s="8"/>
     </row>
@@ -33665,13 +33667,13 @@
         <v>-79.958396911621094</v>
       </c>
       <c r="M703" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N703" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O703" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P703" s="8"/>
     </row>
@@ -33713,13 +33715,13 @@
         <v>-79.815399169921875</v>
       </c>
       <c r="M704" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N704" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O704" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P704" s="8"/>
     </row>
@@ -33761,13 +33763,13 @@
         <v>-79.830596923828125</v>
       </c>
       <c r="M705" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N705" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O705" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P705" s="8"/>
     </row>
@@ -33809,13 +33811,13 @@
         <v>-79.922599792480469</v>
       </c>
       <c r="M706" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N706" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O706" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P706" s="8"/>
     </row>
@@ -33857,13 +33859,13 @@
         <v>-79.8551025390625</v>
       </c>
       <c r="M707" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N707" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O707" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P707" s="8"/>
     </row>
@@ -33905,13 +33907,13 @@
         <v>-79.839500427246094</v>
       </c>
       <c r="M708" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N708" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O708" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P708" s="8"/>
     </row>
@@ -33953,13 +33955,13 @@
         <v>-79.961097717285156</v>
       </c>
       <c r="M709" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N709" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O709" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P709" s="8"/>
     </row>
@@ -34001,13 +34003,13 @@
         <v>-79.789299011230469</v>
       </c>
       <c r="M710" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N710" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O710" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P710" s="8"/>
     </row>
@@ -34049,13 +34051,13 @@
         <v>-79.737701416015625</v>
       </c>
       <c r="M711" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N711" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O711" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P711" s="8"/>
     </row>
@@ -34097,13 +34099,13 @@
         <v>-79.902099609375</v>
       </c>
       <c r="M712" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N712" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O712" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P712" s="8"/>
     </row>
@@ -34145,13 +34147,13 @@
         <v>-79.962799072265625</v>
       </c>
       <c r="M713" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N713" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O713" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P713" s="8"/>
     </row>
@@ -34193,13 +34195,13 @@
         <v>-80.023902893066406</v>
       </c>
       <c r="M714" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N714" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O714" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P714" s="8"/>
     </row>
@@ -34241,13 +34243,13 @@
         <v>-80.040000915527344</v>
       </c>
       <c r="M715" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N715" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O715" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P715" s="8"/>
     </row>
@@ -34289,13 +34291,13 @@
         <v>-80.000198364257813</v>
       </c>
       <c r="M716" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N716" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O716" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P716" s="8"/>
     </row>
@@ -34337,13 +34339,13 @@
         <v>-80.071998596191406</v>
       </c>
       <c r="M717" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N717" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O717" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P717" s="8"/>
     </row>
@@ -34385,13 +34387,13 @@
         <v>-80.043403625488281</v>
       </c>
       <c r="M718" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N718" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O718" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P718" s="8"/>
     </row>
@@ -34433,13 +34435,13 @@
         <v>-79.994499206542969</v>
       </c>
       <c r="M719" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N719" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O719" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P719" s="8"/>
     </row>
@@ -34481,13 +34483,13 @@
         <v>-80.0791015625</v>
       </c>
       <c r="M720" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N720" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O720" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P720" s="8"/>
     </row>
@@ -34529,13 +34531,13 @@
         <v>-79.942497253417969</v>
       </c>
       <c r="M721" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N721" s="8" t="s">
         <v>379</v>
       </c>
       <c r="O721" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P721" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-26-2020 02-08-29
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23223"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2CA4FBA9-7EC7-4C29-9788-AC2E9E57EA69}"/>
+  <xr:revisionPtr revIDLastSave="569" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78745A3F-93DC-493B-A98D-5C0E85DDFE7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOCALIZACION" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="798">
   <si>
     <t>Id_Prov</t>
   </si>
@@ -2436,6 +2436,24 @@
   </si>
   <si>
     <t>A partir del lunes 24 de agosto se dará la apertura de las empresas de bienes y raíces a nivel nacional, así como las ventas y comercio al por mayor.</t>
+  </si>
+  <si>
+    <t>Nuevo plan de reapertura: en 3 semanas termina la movilidad por género; en un mes abren los restaurantes y en octubre, los hoteles.</t>
+  </si>
+  <si>
+    <t>https://www.prensa.com/sociedad/gabinete-aprueba-el-plan-de-reapertura-nacional-y-provincial/</t>
+  </si>
+  <si>
+    <t>Se establece que desde el 14 de septiembre, el toque de queda será de 11:00 p.m. a 5:00 a.m. de lunes a sábado.</t>
+  </si>
+  <si>
+    <t>Minsa entrega nuevo plan de reapertura (Hilo)</t>
+  </si>
+  <si>
+    <t>https://twitter.com/MINSAPma/status/1298409139463479296</t>
+  </si>
+  <si>
+    <t>Detalla nuevo plan de reapertura y da información con respecto al levantamiento de la restricción de movilidad por género y toques de queda.</t>
   </si>
 </sst>
 </file>
@@ -3559,8 +3577,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F22" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F24" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EA6FFEBC-DF5B-4039-8DBA-5ADF7C795E14}" name="Fuente" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{B604F324-ACB1-4871-8569-DD6561328939}" name="Tipo Fuente" dataDxfId="4"/>
@@ -3872,8 +3890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE435327-D82B-436B-B387-4B676AA50241}">
   <dimension ref="A10:P721"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="E191" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N73" sqref="N73:N214"/>
     </sheetView>
   </sheetViews>
@@ -35095,10 +35113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789927B8-B4AE-4E15-AA25-E1A61CBEA5D5}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35549,6 +35567,46 @@
       </c>
       <c r="F22" s="11" t="s">
         <v>791</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75">
+      <c r="A23" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>793</v>
+      </c>
+      <c r="E23" s="13">
+        <v>44068</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="90">
+      <c r="A24" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>796</v>
+      </c>
+      <c r="E24" s="13">
+        <v>44068</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>797</v>
       </c>
     </row>
   </sheetData>
@@ -35574,10 +35632,12 @@
     <hyperlink ref="D20" r:id="rId19" xr:uid="{D21A9D35-5C99-4E0A-97F5-7E5471B3B7CB}"/>
     <hyperlink ref="D21" r:id="rId20" xr:uid="{9A12720B-251E-4C78-B497-CAC093DB4754}"/>
     <hyperlink ref="D22" r:id="rId21" xr:uid="{06B4A1FA-F4C6-4EBB-B7D8-939F7E17F75A}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{C336E5FE-C63F-4912-9211-4B3D0E9ADABA}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{3767A7B8-7E58-4001-ABDE-7843AD67B5DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-26-2020 03-39-08
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="569" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78745A3F-93DC-493B-A98D-5C0E85DDFE7A}"/>
+  <xr:revisionPtr revIDLastSave="573" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{355753BC-D8E9-4E44-968C-C5909EEAEA94}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2429,7 +2429,7 @@
 Domingos: cuarentena total hasta el lunes a las 5:00 a.m.</t>
   </si>
   <si>
-    <t>Gobierno de Panamá vuelve a flexibilizar las medidas de movilidad</t>
+    <t>Gobierno de Panamá vuelve a flexibilizar las medidas de movilidad.</t>
   </si>
   <si>
     <t>https://www.laestrella.com.pa/nacional/200818/gobierno-panama-vuelve-flexibilizar-medidas-movilidad</t>
@@ -2447,7 +2447,7 @@
     <t>Se establece que desde el 14 de septiembre, el toque de queda será de 11:00 p.m. a 5:00 a.m. de lunes a sábado.</t>
   </si>
   <si>
-    <t>Minsa entrega nuevo plan de reapertura (Hilo)</t>
+    <t>MINSA entrega nuevo plan de reapertura (Hilo)</t>
   </si>
   <si>
     <t>https://twitter.com/MINSAPma/status/1298409139463479296</t>
@@ -35115,8 +35115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789927B8-B4AE-4E15-AA25-E1A61CBEA5D5}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35549,7 +35549,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="90">
+    <row r="22" spans="1:6">
       <c r="A22" s="9" t="s">
         <v>734</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-29-2020 15-40-06
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23322"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="631" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B4C8397B-9BCD-438E-9EFA-C6909ECF7870}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2FE5CFF-6308-4C27-90E2-8FEEC3656FB5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2917" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="813">
   <si>
     <t>Id_Prov</t>
   </si>
@@ -2491,6 +2491,15 @@
   </si>
   <si>
     <t>A partir del lunes 21 de septiembre se reactivan las actividades deportivas federativas de lunes a sábados, sin asistencia de público y respetando el toque de queda de cada área.</t>
+  </si>
+  <si>
+    <t>Actividades económicas que se reactivaran a partir del lunes 28 de Septiembre.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/MINSAPma/status/1310392461081145344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conoce las actividades económicas que se reactivarán, cumpliendo con las nuevas regulaciones, a partir de este lunes 28 de septiembre. Sigue las medidas de prevención para evitar el contagio de #COVID19. </t>
   </si>
 </sst>
 </file>
@@ -3650,8 +3659,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F28" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F29" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EA6FFEBC-DF5B-4039-8DBA-5ADF7C795E14}" name="Fuente" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{B604F324-ACB1-4871-8569-DD6561328939}" name="Tipo Fuente" dataDxfId="4"/>
@@ -3964,7 +3973,7 @@
   <dimension ref="A10:P721"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -35251,10 +35260,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789927B8-B4AE-4E15-AA25-E1A61CBEA5D5}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F28" sqref="A28:F28"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35825,6 +35834,26 @@
       </c>
       <c r="F28" s="11" t="s">
         <v>809</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="150">
+      <c r="A29" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="E29" s="13">
+        <v>44101</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -35856,10 +35885,11 @@
     <hyperlink ref="D26" r:id="rId25" xr:uid="{8400FB9F-FF5F-4BAE-8783-EEE32E167476}"/>
     <hyperlink ref="D27" r:id="rId26" xr:uid="{79371927-7668-43BF-8FDE-022CEA0F7117}"/>
     <hyperlink ref="D28" r:id="rId27" xr:uid="{E87FC0F0-FD6E-44B9-8294-63191EC34DCA}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{E83F18A8-D1FE-485F-A0A4-FBA5A2E337FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-05-2020 22-43-10
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23330"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="639" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2FE5CFF-6308-4C27-90E2-8FEEC3656FB5}"/>
+  <xr:revisionPtr revIDLastSave="647" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF69EAE7-9965-46B8-9A96-DBF26FCD85A7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="816">
   <si>
     <t>Id_Prov</t>
   </si>
@@ -2500,6 +2500,15 @@
   </si>
   <si>
     <t xml:space="preserve">Conoce las actividades económicas que se reactivarán, cumpliendo con las nuevas regulaciones, a partir de este lunes 28 de septiembre. Sigue las medidas de prevención para evitar el contagio de #COVID19. </t>
+  </si>
+  <si>
+    <t>Minsa decretaría cuarentena total sábados y domingo en Soná y Santiago de Veraguas</t>
+  </si>
+  <si>
+    <t>https://www.prensa.com/sociedad/minsa-decretara-cuarentena-total-sabados-y-domingo-en-sona-y-santiago-de-veraguas/</t>
+  </si>
+  <si>
+    <t>El ministro de Salud, Luis Francisco Sucre, anunció que “muy posiblemente” la próxima semana comenzará a regir una cuarentena total los sábados y domingo en los distritos de Soná y Santiago, en la provincia de Veraguas, debido a un aumento de los casos de coronavirus en los últimos días.</t>
   </si>
 </sst>
 </file>
@@ -3659,8 +3668,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F29" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F30" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EA6FFEBC-DF5B-4039-8DBA-5ADF7C795E14}" name="Fuente" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{B604F324-ACB1-4871-8569-DD6561328939}" name="Tipo Fuente" dataDxfId="4"/>
@@ -35260,10 +35269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789927B8-B4AE-4E15-AA25-E1A61CBEA5D5}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35854,6 +35863,26 @@
       </c>
       <c r="F29" s="11" t="s">
         <v>812</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="180">
+      <c r="A30" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="E30" s="13">
+        <v>44107</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -35886,10 +35915,11 @@
     <hyperlink ref="D27" r:id="rId26" xr:uid="{79371927-7668-43BF-8FDE-022CEA0F7117}"/>
     <hyperlink ref="D28" r:id="rId27" xr:uid="{E87FC0F0-FD6E-44B9-8294-63191EC34DCA}"/>
     <hyperlink ref="D29" r:id="rId28" xr:uid="{E83F18A8-D1FE-485F-A0A4-FBA5A2E337FF}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{87A2F2E0-EFAD-4072-9A56-0FE9BE45CB99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-07-2020 15-38-54
</commit_message>
<xml_diff>
--- a/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
+++ b/datacovidpa/00 DATACOVID_PN_CUARENTENA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23405"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="647" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF69EAE7-9965-46B8-9A96-DBF26FCD85A7}"/>
+  <xr:revisionPtr revIDLastSave="654" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF4B7653-F04E-4E64-A269-09165D44E25E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="819">
   <si>
     <t>Id_Prov</t>
   </si>
@@ -2509,6 +2509,15 @@
   </si>
   <si>
     <t>El ministro de Salud, Luis Francisco Sucre, anunció que “muy posiblemente” la próxima semana comenzará a regir una cuarentena total los sábados y domingo en los distritos de Soná y Santiago, en la provincia de Veraguas, debido a un aumento de los casos de coronavirus en los últimos días.</t>
+  </si>
+  <si>
+    <t>Panamá registra 683 casos nuevos de covid-19 y 10 defunciones; establecen horarios escalonados</t>
+  </si>
+  <si>
+    <t>https://www.laestrella.com.pa/nacional/201006/panama-registra-683-casos-nuevos-covid-19-10-defunciones-establecen-horarios-escalonados</t>
+  </si>
+  <si>
+    <t>El sector de la construcción deberá iniciar sus labores a las 7: 00 a.m., la empresa privada a las 8: a.m., las instituciones públicas a las 9:00 a.m. y los centros comerciales a las 10:00 a.m., anunció el ministro de Salud, Luis Francisco Sucre.</t>
   </si>
 </sst>
 </file>
@@ -3668,8 +3677,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F30" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F30" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7C00E8C-D9BC-416F-809A-6033577F14AF}" name="Tabla1" displayName="Tabla1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F31" xr:uid="{4AB5A879-BAE3-440D-9AD2-3BBD481D8D15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EA6FFEBC-DF5B-4039-8DBA-5ADF7C795E14}" name="Fuente" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{B604F324-ACB1-4871-8569-DD6561328939}" name="Tipo Fuente" dataDxfId="4"/>
@@ -35269,10 +35278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789927B8-B4AE-4E15-AA25-E1A61CBEA5D5}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35883,6 +35892,26 @@
       </c>
       <c r="F30" s="11" t="s">
         <v>815</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="135">
+      <c r="A31" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>816</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="E31" s="13">
+        <v>44110</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>818</v>
       </c>
     </row>
   </sheetData>
@@ -35916,10 +35945,11 @@
     <hyperlink ref="D28" r:id="rId27" xr:uid="{E87FC0F0-FD6E-44B9-8294-63191EC34DCA}"/>
     <hyperlink ref="D29" r:id="rId28" xr:uid="{E83F18A8-D1FE-485F-A0A4-FBA5A2E337FF}"/>
     <hyperlink ref="D30" r:id="rId29" xr:uid="{87A2F2E0-EFAD-4072-9A56-0FE9BE45CB99}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{081C2501-5AEA-4057-BA37-9393358E4B6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>